<commit_message>
⬆️ Updating `build.gradle` file
* 🔥 Deleting `Log4J` code and files related
* 🎨 Reformatting all code
* ✨ Adding `Step definitions` classes
* ✨ Adding `.feature` files
* ✨ Adding `Runners` classes
* ✨ Adding `constants`
* ✨ Adding `.xml` files
</commit_message>
<xml_diff>
--- a/PlanDeCalidad.xlsx
+++ b/PlanDeCalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Auto-Screenplay-Soap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EE3516-DAA3-468D-BC3D-750C4D28A9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D5C9E7-CAD8-4136-B797-B720D161A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="893" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
@@ -135,31 +135,6 @@
     <t>Célula 2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Hace parte del alcance:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-1. Validar que se realiza una conversión entre USD y COP.
-2. Revisar la tasa de cambio de COP a USD.
-3. Validar que se realiza una conversión entre USD y otras divisas.
-4. Comprobar que la estructura XML devuelta corresponda con la especificada en ambos servicios.</t>
-    </r>
-  </si>
-  <si>
     <t>Tener una cuenta en Xignite con acceso a los servicios SOAP de conversión de moneda y tasa de cambio.</t>
   </si>
   <si>
@@ -244,59 +219,83 @@
     </r>
   </si>
   <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de marzo en las horas de 10:00 AM a 05:00 PM.</t>
+  </si>
+  <si>
+    <t>Se cae el servicio durante el envío de conversión de moneda.</t>
+  </si>
+  <si>
+    <t>Se cae el servicio durante el envío de tasa de cambio.</t>
+  </si>
+  <si>
+    <t>El servidor de Xignite deja de funcionar.</t>
+  </si>
+  <si>
+    <t>El token de acceso caduca antes de lo previsto.</t>
+  </si>
+  <si>
+    <t>No se reconoce una moneda oficial.</t>
+  </si>
+  <si>
+    <t>Se olvida la cuenta registrada en Xignite.</t>
+  </si>
+  <si>
+    <t>El servicio de cambio de moneda no es compatible con SOAP UI.</t>
+  </si>
+  <si>
+    <t>Se agotan los intentos de petición en la cuenta de Xignite.</t>
+  </si>
+  <si>
+    <t>El servicio de tasa de cambio no es compatible con SOAP UI.</t>
+  </si>
+  <si>
+    <t>Un tipo de moneda en especifico que no está en los servicios de Xignite es requerido por el cliente.</t>
+  </si>
+  <si>
+    <t>La definición WSDL provista por Xignite carece de los servicios requeridos.</t>
+  </si>
+  <si>
+    <t>La tasa de cambio devuelta por el servicio es negativa.</t>
+  </si>
+  <si>
+    <t>Se cambia la versión de los servicios desde Xignite.</t>
+  </si>
+  <si>
+    <t>Faltan dígitos en la tasa de cambio devuelta.</t>
+  </si>
+  <si>
+    <t>Los servicios solo aceptan los tipos de moneda en mayúscula.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hace parte del alcance:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Validar que se realiza una conversión entre USD y COP.
+2. Revisar la tasa de cambio de COP a USD.
+3. Validar que se realiza una conversión entre USD y otras divisas.</t>
+    </r>
+  </si>
+  <si>
     <t>Se probarán las respuestas de las peticiones sin un token de autenticación válido.
-Se probarán las peticiones realizando cambios válidos y no válidos en los campos no obligatorios de Username, Password, Tracer, From, To, Country, Symbol y AsOfDate.
-Se probará la petición de conversión de moneda, realizando cambios válidos y no válidos en el campo Amount.
+Se probarán las peticiones realizando cambios válidos en los campos no obligatorios de From, To, Country, Symbol y AsOfDate.
+Se probará la petición de conversión de moneda, realizando cambios válidos en el campo Amount.
 Se realizará una comprobación de las respuestas recibidas por los servicios.
 Todas las pruebas serán ejecutadas de manera automatizada, y como no se conoce el funcionamiento interno de los servicios de conversión de moneda y tasa de cambio, todas las estrategias de prueba serán de caja negra.</t>
-  </si>
-  <si>
-    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de marzo en las horas de 10:00 AM a 05:00 PM.</t>
-  </si>
-  <si>
-    <t>Se cae el servicio durante el envío de conversión de moneda.</t>
-  </si>
-  <si>
-    <t>Se cae el servicio durante el envío de tasa de cambio.</t>
-  </si>
-  <si>
-    <t>El servidor de Xignite deja de funcionar.</t>
-  </si>
-  <si>
-    <t>El token de acceso caduca antes de lo previsto.</t>
-  </si>
-  <si>
-    <t>No se reconoce una moneda oficial.</t>
-  </si>
-  <si>
-    <t>Se olvida la cuenta registrada en Xignite.</t>
-  </si>
-  <si>
-    <t>El servicio de cambio de moneda no es compatible con SOAP UI.</t>
-  </si>
-  <si>
-    <t>Se agotan los intentos de petición en la cuenta de Xignite.</t>
-  </si>
-  <si>
-    <t>El servicio de tasa de cambio no es compatible con SOAP UI.</t>
-  </si>
-  <si>
-    <t>Un tipo de moneda en especifico que no está en los servicios de Xignite es requerido por el cliente.</t>
-  </si>
-  <si>
-    <t>La definición WSDL provista por Xignite carece de los servicios requeridos.</t>
-  </si>
-  <si>
-    <t>La tasa de cambio devuelta por el servicio es negativa.</t>
-  </si>
-  <si>
-    <t>Se cambia la versión de los servicios desde Xignite.</t>
-  </si>
-  <si>
-    <t>Faltan dígitos en la tasa de cambio devuelta.</t>
-  </si>
-  <si>
-    <t>Los servicios solo aceptan los tipos de moneda en mayúscula.</t>
   </si>
 </sst>
 </file>
@@ -486,11 +485,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1292,32 +1291,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1365,34 +1364,34 @@
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +1434,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1484,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
@@ -1513,15 +1512,15 @@
         <v>24</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>25</v>
@@ -1555,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1589,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>25</v>
@@ -1615,7 +1614,7 @@
         <v>21</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1623,7 +1622,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>19</v>
@@ -1649,7 +1648,7 @@
         <v>21</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -1657,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>25</v>
@@ -1683,7 +1682,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1691,7 +1690,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>19</v>
@@ -1717,7 +1716,7 @@
         <v>21</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
@@ -1725,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>25</v>
@@ -1751,7 +1750,7 @@
         <v>23</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1759,7 +1758,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>19</v>
@@ -1785,7 +1784,7 @@
         <v>21</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1793,7 +1792,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>25</v>
@@ -1819,7 +1818,7 @@
         <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1827,7 +1826,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>19</v>
@@ -1853,7 +1852,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -1861,7 +1860,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>25</v>
@@ -1887,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -1895,7 +1894,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>19</v>
@@ -1921,7 +1920,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -1929,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>25</v>
@@ -1955,15 +1954,15 @@
         <v>23</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>19</v>
@@ -1989,15 +1988,15 @@
         <v>21</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>25</v>
@@ -2023,7 +2022,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
♻️  Refactoring all code
* ✨ Adding new `constants` and `paths`
* ✨ Adding content to `Step definitions`
* ✨ Adding content to `.feature` files
</commit_message>
<xml_diff>
--- a/PlanDeCalidad.xlsx
+++ b/PlanDeCalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Auto-Screenplay-Soap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D5C9E7-CAD8-4136-B797-B720D161A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B4B5D-94F5-42BF-9CE3-72DB7229B606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="893" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
@@ -291,10 +291,9 @@
     </r>
   </si>
   <si>
-    <t>Se probarán las respuestas de las peticiones sin un token de autenticación válido.
-Se probarán las peticiones realizando cambios válidos en los campos no obligatorios de From, To, Country, Symbol y AsOfDate.
-Se probará la petición de conversión de moneda, realizando cambios válidos en el campo Amount.
-Se realizará una comprobación de las respuestas recibidas por los servicios.
+    <t>Se probarán las peticiones realizando cambios válidos en los campos no obligatorios de From, To, Country, Symbol y AsOfDate.
+- Se probará la petición de conversión de moneda, realizando cambios válidos en el campo Amount.
+- Se realizará una comprobación de las respuestas recibidas por los servicios.
 Todas las pruebas serán ejecutadas de manera automatizada, y como no se conoce el funcionamiento interno de los servicios de conversión de moneda y tasa de cambio, todas las estrategias de prueba serán de caja negra.</t>
   </si>
 </sst>

</xml_diff>